<commit_message>
final version of saliva analysis
</commit_message>
<xml_diff>
--- a/Dataframes/Output/structured_data_with_features_cleaned.xlsx
+++ b/Dataframes/Output/structured_data_with_features_cleaned.xlsx
@@ -1252,8 +1252,8 @@
       <c r="BI3">
         <v>13.238</v>
       </c>
-      <c r="BJ3">
-        <v>35.307</v>
+      <c r="BK3">
+        <v>364.056351771112</v>
       </c>
     </row>
     <row r="4" spans="1:64">
@@ -1816,9 +1816,6 @@
       <c r="BE6">
         <v>368.6807876069601</v>
       </c>
-      <c r="BF6">
-        <v>363.1125893556326</v>
-      </c>
       <c r="BG6">
         <v>1.58185</v>
       </c>
@@ -2034,7 +2031,7 @@
     </row>
     <row r="8" spans="1:64">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2225,7 +2222,7 @@
     </row>
     <row r="9" spans="1:64">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -2398,9 +2395,6 @@
       <c r="BG9">
         <v>6.8351</v>
       </c>
-      <c r="BH9">
-        <v>9.5616</v>
-      </c>
       <c r="BI9">
         <v>12.237</v>
       </c>
@@ -2409,14 +2403,11 @@
       </c>
       <c r="BK9">
         <v>5.98</v>
-      </c>
-      <c r="BL9">
-        <v>5.4019</v>
       </c>
     </row>
     <row r="10" spans="1:64">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -2607,7 +2598,7 @@
     </row>
     <row r="11" spans="1:64">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2798,7 +2789,7 @@
     </row>
     <row r="12" spans="1:64">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2989,7 +2980,7 @@
     </row>
     <row r="13" spans="1:64">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -3162,9 +3153,6 @@
       <c r="BG13">
         <v>8.3095</v>
       </c>
-      <c r="BH13">
-        <v>12.3045</v>
-      </c>
       <c r="BI13">
         <v>14.532</v>
       </c>
@@ -3173,14 +3161,11 @@
       </c>
       <c r="BK13">
         <v>34.35963028521249</v>
-      </c>
-      <c r="BL13">
-        <v>7.890499999999999</v>
       </c>
     </row>
     <row r="14" spans="1:64">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -3371,7 +3356,7 @@
     </row>
     <row r="15" spans="1:64">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -3562,7 +3547,7 @@
     </row>
     <row r="16" spans="1:64">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -3753,7 +3738,7 @@
     </row>
     <row r="17" spans="1:64">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -3926,9 +3911,6 @@
       <c r="BG17">
         <v>6.86705</v>
       </c>
-      <c r="BH17">
-        <v>13.106</v>
-      </c>
       <c r="BI17">
         <v>12.8225</v>
       </c>
@@ -3937,14 +3919,11 @@
       </c>
       <c r="BK17">
         <v>75.72246081286436</v>
-      </c>
-      <c r="BL17">
-        <v>6.23895</v>
       </c>
     </row>
     <row r="18" spans="1:64">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4135,7 +4114,7 @@
     </row>
     <row r="19" spans="1:64">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4308,9 +4287,6 @@
       <c r="BG19">
         <v>8.199300000000001</v>
       </c>
-      <c r="BH19">
-        <v>10.983</v>
-      </c>
       <c r="BI19">
         <v>11.965</v>
       </c>
@@ -4319,14 +4295,11 @@
       </c>
       <c r="BK19">
         <v>26.84197085604009</v>
-      </c>
-      <c r="BL19">
-        <v>3.765699999999999</v>
       </c>
     </row>
     <row r="20" spans="1:64">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4517,7 +4490,7 @@
     </row>
     <row r="21" spans="1:64">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4708,7 +4681,7 @@
     </row>
     <row r="22" spans="1:64">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4899,7 +4872,7 @@
     </row>
     <row r="23" spans="1:64">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -5080,6 +5053,9 @@
       </c>
       <c r="BJ23">
         <v>9.51675</v>
+      </c>
+      <c r="BK23">
+        <v>111.0799596430522</v>
       </c>
       <c r="BL23">
         <v>5.6128</v>
@@ -5087,7 +5063,7 @@
     </row>
     <row r="24" spans="1:64">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -5278,7 +5254,7 @@
     </row>
     <row r="25" spans="1:64">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -5469,7 +5445,7 @@
     </row>
     <row r="26" spans="1:64">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -5660,7 +5636,7 @@
     </row>
     <row r="27" spans="1:64">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -5851,7 +5827,7 @@
     </row>
     <row r="28" spans="1:64">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -6042,7 +6018,7 @@
     </row>
     <row r="29" spans="1:64">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -6215,9 +6191,6 @@
       <c r="BG29">
         <v>6.526149999999999</v>
       </c>
-      <c r="BH29">
-        <v>10.256</v>
-      </c>
       <c r="BI29">
         <v>11.054</v>
       </c>
@@ -6226,14 +6199,11 @@
       </c>
       <c r="BK29">
         <v>42.55816960813529</v>
-      </c>
-      <c r="BL29">
-        <v>8.84385</v>
       </c>
     </row>
     <row r="30" spans="1:64">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>29</v>

</xml_diff>